<commit_message>
Fix school year period and style
</commit_message>
<xml_diff>
--- a/facture.xlsx
+++ b/facture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WebDev\facture\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA50FD-C5B8-4735-BCF5-1F66F7C15538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3A7C62-270D-46CA-9054-A3FE13EA8051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t xml:space="preserve"> Prestation suivant convention d'application</t>
   </si>
   <si>
-    <t xml:space="preserve"> du projet éducatif territorial TAP 2021-2022</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;&lt; ATELIER ART CREATIF ENFANTS&gt;&gt;</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>MONTANT TOTAL TTC €</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> du projet éducatif territorial TAP 2022-2023</t>
   </si>
 </sst>
 </file>
@@ -1185,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
@@ -1432,7 +1432,7 @@
       <c r="A21" s="31"/>
       <c r="B21" s="79"/>
       <c r="C21" s="75" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D21" s="80"/>
       <c r="E21" s="81"/>
@@ -1454,7 +1454,7 @@
       <c r="A23" s="31"/>
       <c r="B23" s="85"/>
       <c r="C23" s="86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="80"/>
       <c r="E23" s="81"/>
@@ -1479,7 +1479,7 @@
       <c r="A25" s="31"/>
       <c r="B25" s="79"/>
       <c r="C25" s="88" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="76"/>
       <c r="E25" s="77"/>
@@ -1491,7 +1491,7 @@
       <c r="A26" s="31"/>
       <c r="B26" s="79"/>
       <c r="C26" s="87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="76"/>
       <c r="E26" s="81"/>
@@ -1503,7 +1503,7 @@
       <c r="A27" s="31"/>
       <c r="B27" s="79"/>
       <c r="C27" s="87" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="76"/>
       <c r="E27" s="81"/>
@@ -1535,7 +1535,7 @@
       <c r="A30" s="31"/>
       <c r="B30" s="85"/>
       <c r="C30" s="88" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="80"/>
       <c r="E30" s="77">
@@ -1547,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="73">
-        <f t="shared" ref="G30:G41" si="2">IF(ISBLANK(C30),"",(E30*F30))</f>
+        <f t="shared" ref="G30:G40" si="2">IF(ISBLANK(C30),"",(E30*F30))</f>
         <v>27</v>
       </c>
       <c r="H30" s="14"/>
@@ -1556,7 +1556,7 @@
       <c r="A31" s="31"/>
       <c r="B31" s="91"/>
       <c r="C31" s="88" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="80"/>
       <c r="E31" s="77">
@@ -1577,7 +1577,7 @@
       <c r="A32" s="31"/>
       <c r="B32" s="85"/>
       <c r="C32" s="88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="80"/>
       <c r="E32" s="77">
@@ -1598,7 +1598,7 @@
       <c r="A33" s="31"/>
       <c r="B33" s="92"/>
       <c r="C33" s="88" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="76"/>
       <c r="E33" s="77">
@@ -1620,7 +1620,7 @@
       <c r="A34" s="31"/>
       <c r="B34" s="90"/>
       <c r="C34" s="88" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="80"/>
       <c r="E34" s="77">
@@ -1641,7 +1641,7 @@
       <c r="A35" s="31"/>
       <c r="B35" s="91"/>
       <c r="C35" s="88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="80"/>
       <c r="E35" s="77">
@@ -1662,7 +1662,7 @@
       <c r="A36" s="31"/>
       <c r="B36" s="92"/>
       <c r="C36" s="88" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="76"/>
       <c r="E36" s="77">
@@ -1683,7 +1683,7 @@
       <c r="A37" s="31"/>
       <c r="B37" s="92"/>
       <c r="C37" s="88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="76"/>
       <c r="E37" s="77">
@@ -1704,7 +1704,7 @@
       <c r="A38" s="31"/>
       <c r="B38" s="92"/>
       <c r="C38" s="88" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="76"/>
       <c r="E38" s="77">
@@ -1725,7 +1725,7 @@
       <c r="A39" s="31"/>
       <c r="B39" s="90"/>
       <c r="C39" s="88" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="80"/>
       <c r="E39" s="77">
@@ -1746,7 +1746,7 @@
       <c r="A40" s="31"/>
       <c r="B40" s="85"/>
       <c r="C40" s="88" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="80"/>
       <c r="E40" s="77">
@@ -1767,7 +1767,7 @@
       <c r="A41" s="31"/>
       <c r="B41" s="85"/>
       <c r="C41" s="88" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" s="80"/>
       <c r="E41" s="77">
@@ -1838,7 +1838,7 @@
       <c r="C45" s="103"/>
       <c r="D45" s="104"/>
       <c r="E45" s="105" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F45" s="106"/>
       <c r="G45" s="107">
@@ -1860,12 +1860,12 @@
     <row r="47" spans="1:10" ht="20.7" customHeight="1">
       <c r="A47" s="31"/>
       <c r="B47" s="110" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47" s="111"/>
       <c r="D47" s="112"/>
       <c r="E47" s="113" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F47" s="114"/>
       <c r="G47" s="107">
@@ -1879,7 +1879,7 @@
       <c r="C48" s="97"/>
       <c r="D48" s="97"/>
       <c r="E48" s="105" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F48" s="106"/>
       <c r="G48" s="115">
@@ -1891,7 +1891,7 @@
     <row r="49" spans="1:8">
       <c r="A49" s="31"/>
       <c r="B49" s="116" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" s="117"/>
       <c r="D49" s="118"/>
@@ -1903,12 +1903,12 @@
     <row r="50" spans="1:8" ht="20.7" customHeight="1">
       <c r="A50" s="31"/>
       <c r="B50" s="119" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C50" s="120"/>
       <c r="D50" s="120"/>
       <c r="E50" s="105" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F50" s="106"/>
       <c r="G50" s="107">
@@ -1930,12 +1930,12 @@
     <row r="52" spans="1:8" ht="20.7" customHeight="1">
       <c r="A52" s="122"/>
       <c r="B52" s="123" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C52" s="124"/>
       <c r="D52" s="125"/>
       <c r="E52" s="126" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F52" s="127"/>
       <c r="G52" s="107">

</xml_diff>